<commit_message>
edited prediction years to 2021
</commit_message>
<xml_diff>
--- a/FrancePredictions/ Bandol.xlsx
+++ b/FrancePredictions/ Bandol.xlsx
@@ -426,7 +426,7 @@
         <v>1</v>
       </c>
       <c r="F2">
-        <v>13.65909085392952</v>
+        <v>9.891639143228531</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -446,7 +446,7 @@
         <v>0.8660254037844387</v>
       </c>
       <c r="F3">
-        <v>14.45136955738068</v>
+        <v>10.36087130308151</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -466,7 +466,7 @@
         <v>0.5000000000000001</v>
       </c>
       <c r="F4">
-        <v>16.3304124045372</v>
+        <v>11.8361004948616</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -486,7 +486,7 @@
         <v>6.123233995736766e-17</v>
       </c>
       <c r="F5">
-        <v>19.22892391562462</v>
+        <v>14.00294080972671</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -506,7 +506,7 @@
         <v>-0.4999999999999998</v>
       </c>
       <c r="F6">
-        <v>22.62414391517639</v>
+        <v>16.68157880306244</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -526,7 +526,7 @@
         <v>-0.8660254037844385</v>
       </c>
       <c r="F7">
-        <v>25.83943989038468</v>
+        <v>19.6415261387825</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -546,7 +546,7 @@
         <v>-1</v>
       </c>
       <c r="F8">
-        <v>28.29550400257111</v>
+        <v>21.28996098041534</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -566,7 +566,7 @@
         <v>-0.8660254037844388</v>
       </c>
       <c r="F9">
-        <v>28.71917888164521</v>
+        <v>20.12264679670334</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -586,7 +586,7 @@
         <v>-0.5000000000000004</v>
       </c>
       <c r="F10">
-        <v>26.55417495131493</v>
+        <v>17.33410066366196</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -606,7 +606,7 @@
         <v>-1.83697019872103e-16</v>
       </c>
       <c r="F11">
-        <v>21.82583780884743</v>
+        <v>13.82261809110642</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -626,7 +626,7 @@
         <v>0.4999999999999993</v>
       </c>
       <c r="F12">
-        <v>16.94119448900223</v>
+        <v>11.3167012989521</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -646,7 +646,7 @@
         <v>0.8660254037844384</v>
       </c>
       <c r="F13">
-        <v>14.75320385336876</v>
+        <v>10.2355012357235</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -666,7 +666,7 @@
         <v>1</v>
       </c>
       <c r="F14">
-        <v>13.90515195012093</v>
+        <v>9.879003047943115</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -686,7 +686,7 @@
         <v>0.8660254037844387</v>
       </c>
       <c r="F15">
-        <v>14.36316948235035</v>
+        <v>10.67941368222237</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -706,7 +706,7 @@
         <v>0.5000000000000001</v>
       </c>
       <c r="F16">
-        <v>15.93130208492279</v>
+        <v>12.1199037194252</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -726,7 +726,7 @@
         <v>6.123233995736766e-17</v>
       </c>
       <c r="F17">
-        <v>18.41252771139145</v>
+        <v>13.99530737400055</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -746,7 +746,7 @@
         <v>-0.4999999999999998</v>
       </c>
       <c r="F18">
-        <v>21.45673301577568</v>
+        <v>16.21080392599106</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -766,7 +766,7 @@
         <v>-0.8660254037844385</v>
       </c>
       <c r="F19">
-        <v>24.24482103347779</v>
+        <v>17.93669948577881</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -786,7 +786,7 @@
         <v>-1</v>
       </c>
       <c r="F20">
-        <v>26.37406552910805</v>
+        <v>18.54963983297348</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -806,7 +806,7 @@
         <v>-0.8660254037844388</v>
       </c>
       <c r="F21">
-        <v>26.66210149049759</v>
+        <v>17.42080775499344</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -826,7 +826,7 @@
         <v>-0.5000000000000004</v>
       </c>
       <c r="F22">
-        <v>24.59827614307404</v>
+        <v>15.31175798177719</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -846,7 +846,7 @@
         <v>-1.83697019872103e-16</v>
       </c>
       <c r="F23">
-        <v>21.17280341982842</v>
+        <v>13.10456585884094</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -866,7 +866,7 @@
         <v>0.4999999999999993</v>
       </c>
       <c r="F24">
-        <v>17.51768980264664</v>
+        <v>11.64428151845932</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -886,7 +886,7 @@
         <v>0.8660254037844384</v>
       </c>
       <c r="F25">
-        <v>14.96133728027344</v>
+        <v>10.76767483949661</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -906,7 +906,7 @@
         <v>1</v>
       </c>
       <c r="F26">
-        <v>13.95530338704586</v>
+        <v>10.35594524741173</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -926,7 +926,7 @@
         <v>0.8660254037844387</v>
       </c>
       <c r="F27">
-        <v>14.12102606654167</v>
+        <v>11.01092126965523</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -946,7 +946,7 @@
         <v>0.5000000000000001</v>
       </c>
       <c r="F28">
-        <v>15.37734115839005</v>
+        <v>12.23676578998566</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -966,7 +966,7 @@
         <v>6.123233995736766e-17</v>
       </c>
       <c r="F29">
-        <v>17.50256738543511</v>
+        <v>13.8316814661026</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -986,7 +986,7 @@
         <v>-0.4999999999999998</v>
       </c>
       <c r="F30">
-        <v>20.13555759906769</v>
+        <v>15.30383940935135</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1006,7 +1006,7 @@
         <v>-0.8660254037844385</v>
       </c>
       <c r="F31">
-        <v>22.66842376232147</v>
+        <v>16.54835612773895</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1026,7 +1026,7 @@
         <v>-1</v>
       </c>
       <c r="F32">
-        <v>24.63162277579308</v>
+        <v>16.68902498483658</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1046,7 +1046,7 @@
         <v>-0.8660254037844388</v>
       </c>
       <c r="F33">
-        <v>25.23990659117699</v>
+        <v>15.93063229322433</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1066,7 +1066,7 @@
         <v>-0.5000000000000004</v>
       </c>
       <c r="F34">
-        <v>23.90833968997002</v>
+        <v>14.5379891872406</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1086,7 +1086,7 @@
         <v>-1.83697019872103e-16</v>
       </c>
       <c r="F35">
-        <v>21.61035026669503</v>
+        <v>13.10927699804306</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1106,7 +1106,7 @@
         <v>0.4999999999999993</v>
       </c>
       <c r="F36">
-        <v>18.64185829401016</v>
+        <v>12.00802515745163</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1126,7 +1126,7 @@
         <v>0.8660254037844384</v>
       </c>
       <c r="F37">
-        <v>15.88754424452782</v>
+        <v>11.31026089787483</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1146,7 +1146,7 @@
         <v>1</v>
       </c>
       <c r="F38">
-        <v>14.27964314281941</v>
+        <v>10.99008926749229</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1166,7 +1166,7 @@
         <v>0.8660254037844387</v>
       </c>
       <c r="F39">
-        <v>14.0007127147913</v>
+        <v>11.37078860998154</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1186,7 +1186,7 @@
         <v>0.5000000000000001</v>
       </c>
       <c r="F40">
-        <v>14.80465767741203</v>
+        <v>12.32919547557831</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1206,7 +1206,7 @@
         <v>6.123233995736766e-17</v>
       </c>
       <c r="F41">
-        <v>16.45195451021194</v>
+        <v>13.47526555657387</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1226,7 +1226,7 @@
         <v>-0.4999999999999998</v>
       </c>
       <c r="F42">
-        <v>18.61697290420532</v>
+        <v>14.61593506336212</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1246,7 +1246,7 @@
         <v>-0.8660254037844385</v>
       </c>
       <c r="F43">
-        <v>20.93569401621819</v>
+        <v>15.45086355209351</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -1266,7 +1266,7 @@
         <v>-1</v>
       </c>
       <c r="F44">
-        <v>23.04180322527886</v>
+        <v>15.52021702528</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -1286,7 +1286,7 @@
         <v>-0.8660254037844388</v>
       </c>
       <c r="F45">
-        <v>24.03569881796837</v>
+        <v>15.08116254210472</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -1306,7 +1306,7 @@
         <v>-0.5000000000000004</v>
       </c>
       <c r="F46">
-        <v>23.80004104018212</v>
+        <v>14.20994863510132</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -1326,7 +1326,7 @@
         <v>-1.83697019872103e-16</v>
       </c>
       <c r="F47">
-        <v>22.29397530317307</v>
+        <v>13.23060195446014</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -1346,7 +1346,7 @@
         <v>0.4999999999999993</v>
       </c>
       <c r="F48">
-        <v>20.00399085998535</v>
+        <v>12.38990760445595</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -1366,7 +1366,7 @@
         <v>0.8660254037844384</v>
       </c>
       <c r="F49">
-        <v>17.44706899523735</v>
+        <v>11.78912883400917</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -1386,7 +1386,7 @@
         <v>1</v>
       </c>
       <c r="F50">
-        <v>15.09576650977135</v>
+        <v>11.52648814320564</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -1406,7 +1406,7 @@
         <v>0.8660254037844387</v>
       </c>
       <c r="F51">
-        <v>14.02893855333328</v>
+        <v>11.73472375869751</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -1426,7 +1426,7 @@
         <v>0.5000000000000001</v>
       </c>
       <c r="F52">
-        <v>14.31648143529892</v>
+        <v>12.35189292430878</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -1446,7 +1446,7 @@
         <v>6.123233995736766e-17</v>
       </c>
       <c r="F53">
-        <v>15.39748378157616</v>
+        <v>13.21577271819115</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -1466,7 +1466,7 @@
         <v>-0.4999999999999998</v>
       </c>
       <c r="F54">
-        <v>17.0880940258503</v>
+        <v>14.07049551010132</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -1486,7 +1486,7 @@
         <v>-0.8660254037844385</v>
       </c>
       <c r="F55">
-        <v>19.29541731953621</v>
+        <v>14.66752423644066</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -1506,7 +1506,7 @@
         <v>-1</v>
       </c>
       <c r="F56">
-        <v>21.40635476231575</v>
+        <v>14.77699332237244</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -1526,7 +1526,7 @@
         <v>-0.8660254037844388</v>
       </c>
       <c r="F57">
-        <v>22.87450729370117</v>
+        <v>14.54809026122093</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -1546,7 +1546,7 @@
         <v>-0.5000000000000004</v>
       </c>
       <c r="F58">
-        <v>23.55860831618309</v>
+        <v>14.01846586465836</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -1566,7 +1566,7 @@
         <v>-1.83697019872103e-16</v>
       </c>
       <c r="F59">
-        <v>22.84505270123482</v>
+        <v>13.34612061977387</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -1586,7 +1586,7 @@
         <v>0.4999999999999993</v>
       </c>
       <c r="F60">
-        <v>21.38396764159203</v>
+        <v>12.70343384742737</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -1606,7 +1606,7 @@
         <v>0.8660254037844384</v>
       </c>
       <c r="F61">
-        <v>19.11183004379273</v>
+        <v>12.21338245272636</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -1626,7 +1626,7 @@
         <v>1</v>
       </c>
       <c r="F62">
-        <v>16.79317467570305</v>
+        <v>11.96641364097595</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -1646,7 +1646,7 @@
         <v>0.8660254037844387</v>
       </c>
       <c r="F63">
-        <v>14.68785439372063</v>
+        <v>12.04066054224968</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -1666,7 +1666,7 @@
         <v>0.5000000000000001</v>
       </c>
       <c r="F64">
-        <v>14.122918176651</v>
+        <v>12.4623919069767</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -1686,7 +1686,7 @@
         <v>6.123233995736766e-17</v>
       </c>
       <c r="F65">
-        <v>14.5588950586319</v>
+        <v>13.06974229812622</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -1706,7 +1706,7 @@
         <v>-0.4999999999999998</v>
       </c>
       <c r="F66">
-        <v>15.83062578558922</v>
+        <v>13.67847652435303</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -1726,7 +1726,7 @@
         <v>-0.8660254037844385</v>
       </c>
       <c r="F67">
-        <v>17.61821752071381</v>
+        <v>14.11930069923401</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -1746,7 +1746,7 @@
         <v>-1</v>
       </c>
       <c r="F68">
-        <v>19.64703554391861</v>
+        <v>14.26013411283493</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -1766,7 +1766,7 @@
         <v>-0.8660254037844388</v>
       </c>
       <c r="F69">
-        <v>21.57876031160355</v>
+        <v>14.1597319483757</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -1786,7 +1786,7 @@
         <v>-0.5000000000000004</v>
       </c>
       <c r="F70">
-        <v>22.7176817393303</v>
+        <v>13.85013732910156</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -1806,7 +1806,7 @@
         <v>-1.83697019872103e-16</v>
       </c>
       <c r="F71">
-        <v>23.14598630547524</v>
+        <v>13.3988609790802</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -1826,7 +1826,7 @@
         <v>0.4999999999999993</v>
       </c>
       <c r="F72">
-        <v>22.30326623439789</v>
+        <v>12.92597382068634</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -1846,7 +1846,7 @@
         <v>0.8660254037844384</v>
       </c>
       <c r="F73">
-        <v>20.78293406605721</v>
+        <v>12.53632600903511</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -1866,7 +1866,7 @@
         <v>1</v>
       </c>
       <c r="F74">
-        <v>18.61142280220986</v>
+        <v>12.3083705663681</v>
       </c>
     </row>
     <row r="75" spans="1:6">
@@ -1886,7 +1886,7 @@
         <v>0.8660254037844387</v>
       </c>
       <c r="F75">
-        <v>16.3858292722702</v>
+        <v>12.29182554483414</v>
       </c>
     </row>
     <row r="76" spans="1:6">
@@ -1906,7 +1906,7 @@
         <v>0.5000000000000001</v>
       </c>
       <c r="F76">
-        <v>14.51615230441094</v>
+        <v>12.56682641506195</v>
       </c>
     </row>
     <row r="77" spans="1:6">
@@ -1926,7 +1926,7 @@
         <v>6.123233995736766e-17</v>
       </c>
       <c r="F77">
-        <v>14.21516413271427</v>
+        <v>12.98061012625694</v>
       </c>
     </row>
     <row r="78" spans="1:6">
@@ -1946,7 +1946,7 @@
         <v>-0.4999999999999998</v>
       </c>
       <c r="F78">
-        <v>14.82783898472786</v>
+        <v>13.41162049174309</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -1966,7 +1966,7 @@
         <v>-0.8660254037844385</v>
       </c>
       <c r="F79">
-        <v>16.12790797233582</v>
+        <v>13.7455205321312</v>
       </c>
     </row>
     <row r="80" spans="1:6">
@@ -1986,7 +1986,7 @@
         <v>-1</v>
       </c>
       <c r="F80">
-        <v>17.95100011110306</v>
+        <v>13.89438174962998</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -2006,7 +2006,7 @@
         <v>-0.8660254037844388</v>
       </c>
       <c r="F81">
-        <v>19.81865611076355</v>
+        <v>13.87261844277382</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -2026,7 +2026,7 @@
         <v>-0.5000000000000004</v>
       </c>
       <c r="F82">
-        <v>21.60705123662949</v>
+        <v>13.70437644124031</v>
       </c>
     </row>
     <row r="83" spans="1:6">
@@ -2046,7 +2046,7 @@
         <v>-1.83697019872103e-16</v>
       </c>
       <c r="F83">
-        <v>22.65574044466019</v>
+        <v>13.41258300542831</v>
       </c>
     </row>
     <row r="84" spans="1:6">
@@ -2066,7 +2066,7 @@
         <v>0.4999999999999993</v>
       </c>
       <c r="F84">
-        <v>22.86390411376953</v>
+        <v>13.07547482252121</v>
       </c>
     </row>
     <row r="85" spans="1:6">
@@ -2086,7 +2086,7 @@
         <v>0.8660254037844384</v>
       </c>
       <c r="F85">
-        <v>21.95287873625756</v>
+        <v>12.77330368757248</v>
       </c>
     </row>
     <row r="86" spans="1:6">
@@ -2106,7 +2106,7 @@
         <v>1</v>
       </c>
       <c r="F86">
-        <v>20.37910727739334</v>
+        <v>12.56985723376274</v>
       </c>
     </row>
     <row r="87" spans="1:6">
@@ -2126,7 +2126,7 @@
         <v>0.8660254037844387</v>
       </c>
       <c r="F87">
-        <v>18.25763634324074</v>
+        <v>12.51929370164871</v>
       </c>
     </row>
     <row r="88" spans="1:6">
@@ -2146,7 +2146,7 @@
         <v>0.5000000000000001</v>
       </c>
       <c r="F88">
-        <v>16.11081323742867</v>
+        <v>12.66268625259399</v>
       </c>
     </row>
     <row r="89" spans="1:6">
@@ -2166,7 +2166,7 @@
         <v>6.123233995736766e-17</v>
       </c>
       <c r="F89">
-        <v>14.41907351255417</v>
+        <v>12.93439031839371</v>
       </c>
     </row>
     <row r="90" spans="1:6">
@@ -2186,7 +2186,7 @@
         <v>-0.4999999999999998</v>
       </c>
       <c r="F90">
-        <v>14.28042155086994</v>
+        <v>13.23629688620567</v>
       </c>
     </row>
     <row r="91" spans="1:6">
@@ -2206,7 +2206,7 @@
         <v>-0.8660254037844385</v>
       </c>
       <c r="F91">
-        <v>15.00834287047386</v>
+        <v>13.48900035023689</v>
       </c>
     </row>
     <row r="92" spans="1:6">
@@ -2226,7 +2226,7 @@
         <v>-1</v>
       </c>
       <c r="F92">
-        <v>16.32170133471489</v>
+        <v>13.62997987866402</v>
       </c>
     </row>
     <row r="93" spans="1:6">
@@ -2246,7 +2246,7 @@
         <v>-0.8660254037844388</v>
       </c>
       <c r="F93">
-        <v>18.16651658058167</v>
+        <v>13.65535491704941</v>
       </c>
     </row>
     <row r="94" spans="1:6">
@@ -2266,7 +2266,7 @@
         <v>-0.5000000000000004</v>
       </c>
       <c r="F94">
-        <v>20.02604794621468</v>
+        <v>13.57781972289085</v>
       </c>
     </row>
     <row r="95" spans="1:6">
@@ -2286,7 +2286,7 @@
         <v>-1.83697019872103e-16</v>
       </c>
       <c r="F95">
-        <v>21.67271232247353</v>
+        <v>13.39948019385338</v>
       </c>
     </row>
     <row r="96" spans="1:6">
@@ -2306,7 +2306,7 @@
         <v>0.4999999999999993</v>
       </c>
       <c r="F96">
-        <v>22.63693768262863</v>
+        <v>13.16799955368042</v>
       </c>
     </row>
     <row r="97" spans="1:6">
@@ -2326,7 +2326,7 @@
         <v>0.8660254037844384</v>
       </c>
       <c r="F97">
-        <v>22.6779540014267</v>
+        <v>12.94052075743675</v>
       </c>
     </row>
     <row r="98" spans="1:6">
@@ -2346,7 +2346,7 @@
         <v>1</v>
       </c>
       <c r="F98">
-        <v>21.72972676753998</v>
+        <v>12.77031826376915</v>
       </c>
     </row>
     <row r="99" spans="1:6">
@@ -2366,7 +2366,7 @@
         <v>0.8660254037844387</v>
       </c>
       <c r="F99">
-        <v>20.09025214672089</v>
+        <v>12.70114566087723</v>
       </c>
     </row>
     <row r="100" spans="1:6">
@@ -2386,7 +2386,7 @@
         <v>0.5000000000000001</v>
       </c>
       <c r="F100">
-        <v>17.99212556481362</v>
+        <v>12.74653133749962</v>
       </c>
     </row>
     <row r="101" spans="1:6">
@@ -2406,7 +2406,7 @@
         <v>6.123233995736766e-17</v>
       </c>
       <c r="F101">
-        <v>15.89696666359902</v>
+        <v>12.91738070845604</v>
       </c>
     </row>
     <row r="102" spans="1:6">
@@ -2426,7 +2426,7 @@
         <v>-0.4999999999999998</v>
       </c>
       <c r="F102">
-        <v>14.36497218072414</v>
+        <v>13.12456869482994</v>
       </c>
     </row>
     <row r="103" spans="1:6">
@@ -2446,7 +2446,7 @@
         <v>-0.8660254037844385</v>
       </c>
       <c r="F103">
-        <v>14.33278198361397</v>
+        <v>13.31404345035553</v>
       </c>
     </row>
     <row r="104" spans="1:6">
@@ -2466,7 +2466,7 @@
         <v>-1</v>
       </c>
       <c r="F104">
-        <v>15.14644455552101</v>
+        <v>13.43940713405609</v>
       </c>
     </row>
     <row r="105" spans="1:6">
@@ -2486,7 +2486,7 @@
         <v>-0.8660254037844388</v>
       </c>
       <c r="F105">
-        <v>16.50325843811035</v>
+        <v>13.49265109300613</v>
       </c>
     </row>
     <row r="106" spans="1:6">
@@ -2506,7 +2506,7 @@
         <v>-0.5000000000000004</v>
       </c>
       <c r="F106">
-        <v>18.35484530806542</v>
+        <v>13.47234467864036</v>
       </c>
     </row>
     <row r="107" spans="1:6">
@@ -2526,7 +2526,7 @@
         <v>-1.83697019872103e-16</v>
       </c>
       <c r="F107">
-        <v>20.20279653906822</v>
+        <v>13.37295964360237</v>
       </c>
     </row>
     <row r="108" spans="1:6">
@@ -2546,7 +2546,7 @@
         <v>0.4999999999999993</v>
       </c>
       <c r="F108">
-        <v>21.74540274858475</v>
+        <v>13.22127188444138</v>
       </c>
     </row>
     <row r="109" spans="1:6">
@@ -2566,7 +2566,7 @@
         <v>0.8660254037844384</v>
       </c>
       <c r="F109">
-        <v>22.6350784444809</v>
+        <v>13.05642740726471</v>
       </c>
     </row>
     <row r="110" spans="1:6">
@@ -2586,7 +2586,7 @@
         <v>1</v>
       </c>
       <c r="F110">
-        <v>22.53964851021767</v>
+        <v>12.91924899220467</v>
       </c>
     </row>
     <row r="111" spans="1:6">
@@ -2606,7 +2606,7 @@
         <v>0.8660254037844387</v>
       </c>
       <c r="F111">
-        <v>21.55194468021393</v>
+        <v>12.84126339554787</v>
       </c>
     </row>
     <row r="112" spans="1:6">
@@ -2626,7 +2626,7 @@
         <v>0.5000000000000001</v>
       </c>
       <c r="F112">
-        <v>19.84967803835869</v>
+        <v>12.84355016350746</v>
       </c>
     </row>
     <row r="113" spans="1:6">
@@ -2646,7 +2646,7 @@
         <v>6.123233995736766e-17</v>
       </c>
       <c r="F113">
-        <v>17.76259512066841</v>
+        <v>12.91958661675453</v>
       </c>
     </row>
     <row r="114" spans="1:6">
@@ -2666,7 +2666,7 @@
         <v>-0.4999999999999998</v>
       </c>
       <c r="F114">
-        <v>15.71001198410988</v>
+        <v>13.05487121343613</v>
       </c>
     </row>
     <row r="115" spans="1:6">
@@ -2686,7 +2686,7 @@
         <v>-0.8660254037844385</v>
       </c>
       <c r="F115">
-        <v>14.34292758584023</v>
+        <v>13.19326181411743</v>
       </c>
     </row>
     <row r="116" spans="1:6">
@@ -2706,7 +2706,7 @@
         <v>-1</v>
       </c>
       <c r="F116">
-        <v>14.4019432759285</v>
+        <v>13.3001391351223</v>
       </c>
     </row>
     <row r="117" spans="1:6">
@@ -2726,7 +2726,7 @@
         <v>-0.8660254037844388</v>
       </c>
       <c r="F117">
-        <v>15.2759022295475</v>
+        <v>13.36885353326798</v>
       </c>
     </row>
     <row r="118" spans="1:6">
@@ -2746,7 +2746,7 @@
         <v>-0.5000000000000004</v>
       </c>
       <c r="F118">
-        <v>16.69017893075943</v>
+        <v>13.38385654687881</v>
       </c>
     </row>
     <row r="119" spans="1:6">
@@ -2766,7 +2766,7 @@
         <v>-1.83697019872103e-16</v>
       </c>
       <c r="F119">
-        <v>18.52958213686943</v>
+        <v>13.33870493769646</v>
       </c>
     </row>
     <row r="120" spans="1:6">
@@ -2786,7 +2786,7 @@
         <v>0.4999999999999993</v>
       </c>
       <c r="F120">
-        <v>20.3612762105465</v>
+        <v>13.24669657349586</v>
       </c>
     </row>
     <row r="121" spans="1:6">
@@ -2806,7 +2806,7 @@
         <v>0.8660254037844384</v>
       </c>
       <c r="F121">
-        <v>21.80757151722908</v>
+        <v>13.13288305401802</v>
       </c>
     </row>
     <row r="122" spans="1:6">
@@ -2826,7 +2826,7 @@
         <v>1</v>
       </c>
       <c r="F122">
-        <v>22.6258953332901</v>
+        <v>13.02604970932007</v>
       </c>
     </row>
     <row r="123" spans="1:6">
@@ -2846,7 +2846,7 @@
         <v>0.8660254037844387</v>
       </c>
       <c r="F123">
-        <v>22.40479063034058</v>
+        <v>12.95219788551331</v>
       </c>
     </row>
     <row r="124" spans="1:6">
@@ -2866,7 +2866,7 @@
         <v>0.5000000000000001</v>
       </c>
       <c r="F124">
-        <v>21.37634397625924</v>
+        <v>12.9273505628109</v>
       </c>
     </row>
     <row r="125" spans="1:6">
@@ -2886,7 +2886,7 @@
         <v>6.123233995736766e-17</v>
       </c>
       <c r="F125">
-        <v>19.61679070949555</v>
+        <v>12.95628342628479</v>
       </c>
     </row>
     <row r="126" spans="1:6">
@@ -2906,7 +2906,7 @@
         <v>-0.4999999999999998</v>
       </c>
       <c r="F126">
-        <v>17.53966668128967</v>
+        <v>13.02703846693039</v>
       </c>
     </row>
     <row r="127" spans="1:6">
@@ -2926,7 +2926,7 @@
         <v>-0.8660254037844385</v>
       </c>
       <c r="F127">
-        <v>15.53249155759812</v>
+        <v>13.11689837574959</v>
       </c>
     </row>
     <row r="128" spans="1:6">
@@ -2946,7 +2946,7 @@
         <v>-1</v>
       </c>
       <c r="F128">
-        <v>14.33214163780213</v>
+        <v>13.20564469099045</v>
       </c>
     </row>
     <row r="129" spans="1:6">
@@ -2966,7 +2966,7 @@
         <v>-0.8660254037844388</v>
       </c>
       <c r="F129">
-        <v>14.48427307605744</v>
+        <v>13.27475913167</v>
       </c>
     </row>
     <row r="130" spans="1:6">
@@ -2986,7 +2986,7 @@
         <v>-0.5000000000000004</v>
       </c>
       <c r="F130">
-        <v>15.406828622818</v>
+        <v>13.30789882540703</v>
       </c>
     </row>
     <row r="131" spans="1:6">
@@ -3006,7 +3006,7 @@
         <v>-1.83697019872103e-16</v>
       </c>
       <c r="F131">
-        <v>16.87213707208634</v>
+        <v>13.29776228666305</v>
       </c>
     </row>
     <row r="132" spans="1:6">
@@ -3026,7 +3026,7 @@
         <v>0.4999999999999993</v>
       </c>
       <c r="F132">
-        <v>18.69483080267906</v>
+        <v>13.24890460968018</v>
       </c>
     </row>
     <row r="133" spans="1:6">
@@ -3046,7 +3046,7 @@
         <v>0.8660254037844384</v>
       </c>
       <c r="F133">
-        <v>20.50733948469162</v>
+        <v>13.17557340860367</v>
       </c>
     </row>
   </sheetData>

</xml_diff>